<commit_message>
sound volume adjusted first person camera fixed mostly
</commit_message>
<xml_diff>
--- a/project/src/main/hunting game chunk layout.xlsx
+++ b/project/src/main/hunting game chunk layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Dropbox\IdeaProjects\CGA_Project\project\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37AF7DF-DEFD-42AA-B579-6E52BB544316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E883668-5094-4ABA-A1C4-0927D9572E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E852BC5A-13BB-418C-9D40-31E59C52D8D7}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <t>STONE</t>
   </si>
   <si>
-    <t>3xACC</t>
+    <t>PILZ</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>